<commit_message>
sherbimi llojet e filtrave dhe kerkimi
</commit_message>
<xml_diff>
--- a/ExcelFiles/LlojetEsherbimitFilter.xlsx
+++ b/ExcelFiles/LlojetEsherbimitFilter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arbi.topi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arbi.topi\IdeaProjects\TestimTemp\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E9C316-7B52-4E7C-A27B-1DA2679D1047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83190BE-01C6-4FA2-B4D8-AE51795A11FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1920" yWindow="-14655" windowWidth="15225" windowHeight="8970" xr2:uid="{ECFBA7A2-F2B3-4998-8097-A7B426BDB62D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Llojet e sherbimit</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Shërbime me vulë</t>
+  </si>
+  <si>
+    <t>ExpectedSherbim</t>
   </si>
 </sst>
 </file>
@@ -440,51 +443,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9302DF3A-65BF-42E8-940B-4B75E972D7DE}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>

</xml_diff>